<commit_message>
added jupiter and csv handlin
</commit_message>
<xml_diff>
--- a/excel/first_list.xlsx
+++ b/excel/first_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Desktop\scrape\wahlscraper\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793AC66E-DEE6-4DC0-ABD8-FCD8019C4516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601CC7D4-33C5-4DAD-9DA5-2E69005A3A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF238402-586B-4987-B9E7-597CF0CCAE7C}"/>
   </bookViews>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:G463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>